<commit_message>
Primer commit al repo de GitHub
</commit_message>
<xml_diff>
--- a/data/Departamental.xlsx
+++ b/data/Departamental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Borrado Rapido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Alejo\Documentos\AlimentosAI\prueba_tecnica_repo_202502\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00F66AF-233A-4C7F-B8B7-449F3D45A633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A2963-96D0-4269-B9E6-A521861DD59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="14745" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,14 +427,15 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" customWidth="1"/>
     <col min="10" max="21" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>